<commit_message>
Test Data generation Konzept
</commit_message>
<xml_diff>
--- a/RayTracerJava/src/test/resources/Daten.xlsx
+++ b/RayTracerJava/src/test/resources/Daten.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\CodingJava\RayTracerJava\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF07529-2055-409E-BCD4-4EE7A820504F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4146668-21F9-49B4-AE88-BE8F2F6DA5F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F9F5DE1C-86AA-4644-9276-A23A54730184}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{F9F5DE1C-86AA-4644-9276-A23A54730184}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>#</t>
   </si>
@@ -52,10 +52,28 @@
     <t>y</t>
   </si>
   <si>
-    <t>z</t>
-  </si>
-  <si>
     <t>xDir</t>
+  </si>
+  <si>
+    <t>Phi</t>
+  </si>
+  <si>
+    <t>yDir</t>
+  </si>
+  <si>
+    <t>zDir</t>
+  </si>
+  <si>
+    <t>xPoint</t>
+  </si>
+  <si>
+    <t>yPoint</t>
+  </si>
+  <si>
+    <t>zPoint</t>
+  </si>
+  <si>
+    <t>Delta</t>
   </si>
 </sst>
 </file>
@@ -411,15 +429,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7EA0B0-B097-4756-B556-864D58B43352}">
-  <dimension ref="A1:F12"/>
+  <sheetPr codeName="Tabelle1"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,193 +446,298 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>89.99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <f>3*C3</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E5" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <f>$C$2*SIN(B4*PI()/180)</f>
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <f>$C$2*COS(B4*PI()/180)</f>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
+      <c r="J5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <f>$C$3*SIN(A6*PI()/180)</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <f>$C$3*COS(A6*PI()/180)</f>
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f>$C$4-$C$3*COS(PI()*$C$2/180)</f>
+        <v>29.998254670756864</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>45</v>
       </c>
-      <c r="C5" s="1">
-        <f t="shared" ref="C5:C12" si="0">$C$2*SIN(B5*PI()/180)</f>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" ref="C7:C14" si="0">$C$3*SIN(A7*PI()/180)</f>
         <v>7.0710678118654746</v>
       </c>
-      <c r="D5" s="1">
-        <f t="shared" ref="D5:D12" si="1">$C$2*COS(B5*PI()/180)</f>
+      <c r="D7" s="1">
+        <f t="shared" ref="D7:D14" si="1">$C$3*COS(A7*PI()/180)</f>
         <v>7.0710678118654755</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>90</v>
       </c>
-      <c r="C6" s="1">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D8" s="1">
         <f t="shared" si="1"/>
         <v>6.1257422745431001E-16</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>135</v>
       </c>
-      <c r="C7" s="1">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
         <f t="shared" si="0"/>
         <v>7.0710678118654755</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D9" s="1">
         <f t="shared" si="1"/>
         <v>-7.0710678118654746</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>180</v>
       </c>
-      <c r="C8" s="1">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
         <f t="shared" si="0"/>
         <v>1.22514845490862E-15</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D10" s="1">
         <f t="shared" si="1"/>
         <v>-10</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>225</v>
       </c>
-      <c r="C9" s="1">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
         <f t="shared" si="0"/>
         <v>-7.0710678118654746</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D11" s="1">
         <f t="shared" si="1"/>
         <v>-7.0710678118654773</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>270</v>
       </c>
-      <c r="C10" s="1">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
         <f t="shared" si="0"/>
         <v>-10</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D12" s="1">
         <f t="shared" si="1"/>
         <v>-1.83772268236293E-15</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>315</v>
       </c>
-      <c r="C11" s="1">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
         <f t="shared" si="0"/>
         <v>-7.0710678118654773</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D13" s="1">
         <f t="shared" si="1"/>
         <v>7.0710678118654737</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>360</v>
       </c>
-      <c r="C12" s="1">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
         <f t="shared" si="0"/>
         <v>-2.45029690981724E-15</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D14" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="E12">
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
         <v>0</v>
       </c>
     </row>

</xml_diff>